<commit_message>
Update excel template, valid existed question
</commit_message>
<xml_diff>
--- a/src/assets/file/employee.xlsx
+++ b/src/assets/file/employee.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>Nguyễn Văn Hải</t>
   </si>
@@ -68,20 +68,29 @@
     <t>Phone</t>
   </si>
   <si>
-    <t>aaaaaaaaaaaa</t>
-  </si>
-  <si>
-    <t>ádsđa@sadas.dsf</t>
-  </si>
-  <si>
-    <t>dsđa@sadas.dsf</t>
+    <t>0931254125</t>
+  </si>
+  <si>
+    <t>0935164589</t>
+  </si>
+  <si>
+    <t>thongnd@gmail.com</t>
+  </si>
+  <si>
+    <t>thongnd121@gmail.com</t>
+  </si>
+  <si>
+    <t>1 Lê Quang Định, Phường 12, Quận Bình Thạnh</t>
+  </si>
+  <si>
+    <t>1 Phan Đăng Lưu, Phường 12, Quận Bình Thạnh</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -95,8 +104,14 @@
       <name val="Times New Roman"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -109,8 +124,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -118,24 +145,67 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="7">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -143,6 +213,130 @@
           <bgColor theme="4"/>
         </patternFill>
       </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -158,14 +352,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F11" totalsRowShown="0" headerRowDxfId="0" dataCellStyle="Normal">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F11" totalsRowShown="0" headerRowDxfId="1" dataCellStyle="Normal">
   <tableColumns count="6">
-    <tableColumn id="1" name="Fullname" dataCellStyle="Normal"/>
-    <tableColumn id="2" name="Email" dataCellStyle="Normal"/>
-    <tableColumn id="3" name="Role" dataCellStyle="Normal"/>
-    <tableColumn id="4" name="Gender" dataCellStyle="Normal"/>
-    <tableColumn id="5" name="Address" dataCellStyle="Normal"/>
-    <tableColumn id="6" name="Phone" dataCellStyle="Normal"/>
+    <tableColumn id="1" name="Fullname" dataDxfId="6" dataCellStyle="Normal"/>
+    <tableColumn id="2" name="Email" dataDxfId="5" dataCellStyle="Normal"/>
+    <tableColumn id="3" name="Role" dataDxfId="4" dataCellStyle="Normal"/>
+    <tableColumn id="4" name="Gender" dataDxfId="3" dataCellStyle="Normal"/>
+    <tableColumn id="5" name="Address" dataDxfId="2" dataCellStyle="Normal"/>
+    <tableColumn id="6" name="Phone" dataDxfId="0" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -434,10 +628,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -446,232 +640,243 @@
     <col min="2" max="2" width="28.375" customWidth="1"/>
     <col min="3" max="3" width="18.375" customWidth="1"/>
     <col min="4" max="4" width="24.875" customWidth="1"/>
-    <col min="5" max="5" width="19.75" customWidth="1"/>
-    <col min="6" max="6" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.125" customWidth="1"/>
+    <col min="6" max="6" width="13" style="9" customWidth="1"/>
+    <col min="9" max="9" width="12.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="8" t="s">
         <v>13</v>
       </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="2">
-        <v>1234516789</v>
+      <c r="H2" s="3"/>
+      <c r="I2" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="2" t="s">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="7"/>
+      <c r="H4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="7"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="2">
-        <v>1234156789</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="H6" t="s">
-        <v>7</v>
-      </c>
-      <c r="I6" t="s">
-        <v>1</v>
-      </c>
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="7"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="I7" t="s">
-        <v>2</v>
-      </c>
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="7"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="7"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="H9" t="s">
-        <v>9</v>
-      </c>
-      <c r="I9" t="s">
-        <v>10</v>
-      </c>
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="7"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="I10" t="s">
-        <v>11</v>
-      </c>
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="7"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="7"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
+      <c r="A12" s="3"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="7"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
+      <c r="A13" s="3"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="7"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
+      <c r="A14" s="3"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="7"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
+      <c r="A15" s="3"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="7"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
+      <c r="A16" s="3"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="7"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
+      <c r="A17" s="3"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="7"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
+      <c r="A18" s="3"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="7"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
+      <c r="A19" s="3"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="7"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
+      <c r="A20" s="3"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="7"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="7"/>
     </row>
   </sheetData>
   <dataConsolidate/>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576">
-      <formula1>$I$6:$I$7</formula1>
+      <formula1>$I$1:$I$2</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
-      <formula1>$I$9:$I$10</formula1>
+      <formula1>$I$4:$I$5</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>

</xml_diff>

<commit_message>
update excel template and gui
</commit_message>
<xml_diff>
--- a/src/assets/file/employee.xlsx
+++ b/src/assets/file/employee.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\New folder (4)\src\assets\file\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7740"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7740" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Guideline" sheetId="1" r:id="rId1"/>
+    <sheet name="Empolyee" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,12 +27,18 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
+    <t>Nguyễn Văn Hải</t>
+  </si>
+  <si>
     <t>Employee</t>
   </si>
   <si>
     <t>Test Owner</t>
   </si>
   <si>
+    <t>Nguyễn Quốc Huy</t>
+  </si>
+  <si>
     <t>Fullname</t>
   </si>
   <si>
@@ -74,23 +81,17 @@
     <t>1 Phan Đăng Lưu, Phường 12, Quận Bình Thạnh</t>
   </si>
   <si>
-    <t>Nguyễn Đình Thông</t>
-  </si>
-  <si>
-    <t>Nguyễn Hồng Anh</t>
-  </si>
-  <si>
-    <t>anhnguyenhong0311@gmail.com</t>
-  </si>
-  <si>
-    <t>thongnd21@gmail.com</t>
+    <t>thongnd@gmail.com</t>
+  </si>
+  <si>
+    <t>thongnd121@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -105,18 +106,10 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
       <sz val="12"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -134,13 +127,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -173,18 +166,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -201,25 +190,13 @@
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="4"/>
         </patternFill>
       </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -228,6 +205,12 @@
         </right>
         <top/>
         <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
   </dxfs>
@@ -520,256 +503,281 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.375" customWidth="1"/>
-    <col min="2" max="2" width="30.875" customWidth="1"/>
-    <col min="3" max="3" width="18.375" customWidth="1"/>
-    <col min="4" max="4" width="10.625" customWidth="1"/>
-    <col min="5" max="5" width="41.25" customWidth="1"/>
-    <col min="6" max="6" width="13" style="1" customWidth="1"/>
-    <col min="9" max="9" width="12.625" customWidth="1"/>
+    <col min="2" max="2" width="12.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="3"/>
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="9" t="s">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="10" t="s">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
+      <c r="B5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="3"/>
-      <c r="I2" s="6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="I3" s="7"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="11"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="13"/>
-      <c r="H4" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="I4" s="8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="13"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="13"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="13"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="11"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="13"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="11"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="13"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="11"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="13"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="13"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="11"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="13"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="11"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="13"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="11"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="13"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="11"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="13"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="11"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="13"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="11"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="13"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="11"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="13"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="11"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="13"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="11"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="13"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="11"/>
-      <c r="B21" s="11"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="13"/>
     </row>
   </sheetData>
   <dataConsolidate/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.25" customWidth="1"/>
+    <col min="2" max="2" width="25" customWidth="1"/>
+    <col min="3" max="3" width="14.25" customWidth="1"/>
+    <col min="4" max="4" width="15.875" customWidth="1"/>
+    <col min="5" max="5" width="20.5" customWidth="1"/>
+    <col min="6" max="6" width="12.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="9"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="9"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="9"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="9"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="9"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="9"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="9"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="9"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="7"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="9"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="7"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="9"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="7"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="9"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="7"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="9"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="7"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="9"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="7"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="9"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="7"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="9"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="7"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="9"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="7"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="9"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="7"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="9"/>
+    </row>
+  </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D21">
+      <formula1>$I$4:$I$5</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C21">
       <formula1>$I$1:$I$2</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
-      <formula1>$I$4:$I$5</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
@@ -777,9 +785,8 @@
     <hyperlink ref="B2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
   <tableParts count="1">
-    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>